<commit_message>
#5 - api 설계
hashtag 의 url 부분 수정
</commit_message>
<xml_diff>
--- a/document/게시판api설계.xlsx
+++ b/document/게시판api설계.xlsx
@@ -5,7 +5,7 @@
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\github\project-board\document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\github\project-board1\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
@@ -21,193 +21,193 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <x:si>
+    <x:t>/sign-up</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/api/articleComments/{article-comment-id}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/api/articles/{article-id}/articleComments</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/api/articles/{article-id}/articlecomments</x:t>
+  </x:si>
+  <x:si>
+    <x:t>id, pw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>에러 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VIEW</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 가입</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시글 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>필터: 본문</x:t>
+  </x:si>
+  <x:si>
+    <x:t>URL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>API</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>종류</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GET</x:t>
+  </x:si>
+  <x:si>
+    <x:t>설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>본문</x:t>
+  </x:si>
+  <x:si>
+    <x:t>필터: 제목, 본문, id, 글쓴이, 해시태그</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/api/articles/{article-id}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/articles/{article-id}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>특정 게시글과 관련된 댓글 단일 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/api/articleComments</x:t>
+  </x:si>
+  <x:si>
+    <x:t>특정 게시글과 관련된 댓글 리스트 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/api/articles/{article-id}/articlecomments{article-comment-id}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>제목, 본문, id, 해시태그</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판 해시태그 검색 전용 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>어떤 데이터가 전달 될지 설계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/articles/search</x:t>
+  </x:si>
+  <x:si>
+    <x:t>루트 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시글id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>POST</x:t>
+  </x:si>
+  <x:si>
+    <x:t>댓글의 id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>댓글 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시글 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DELETE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>METHOD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/error</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 요청</x:t>
+  </x:si>
+  <x:si>
+    <x:t>본문, id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시글 삭제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/login</x:t>
+  </x:si>
+  <x:si>
+    <x:t>댓글 등록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시글 등록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>댓글 삭제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>id, pw, email, nickname, etc.</x:t>
+  </x:si>
+  <x:si>
     <x:t>제목, 본문, 해시태그</x:t>
   </x:si>
   <x:si>
-    <x:t>루트 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/login</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판 해시태그 검색 전용 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GET</x:t>
-  </x:si>
-  <x:si>
-    <x:t>댓글 등록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>종류</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/sign-up</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시글 등록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>특정 게시글과 관련된 댓글 단일 조회</x:t>
-  </x:si>
-  <x:si>
     <x:t>/api/sign-up</x:t>
   </x:si>
   <x:si>
-    <x:t>댓글 삭제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>댓글 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시글id</x:t>
-  </x:si>
-  <x:si>
-    <x:t>POST</x:t>
-  </x:si>
-  <x:si>
-    <x:t>설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>본문, id</x:t>
+    <x:t>게시판 검색 전용 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/api/articles</x:t>
+  </x:si>
+  <x:si>
+    <x:t>댓글 전체 리스트 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시글 전체 리스트 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>댓글 단일 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/articles</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PUT / PATCH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>각 페이지로 이동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EndPoints</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시글 단일 조회</x:t>
   </x:si>
   <x:si>
     <x:t>/api/login</x:t>
   </x:si>
   <x:si>
-    <x:t>댓글 전체 리스트 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시글 삭제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>본문</x:t>
-  </x:si>
-  <x:si>
-    <x:t>METHOD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>댓글의 id</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 요청</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/api/articles/{article-id}/articleComments</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/api/articles/{article-id}/articlecomments</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/api/articleComments/{article-comment-id}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>URL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시글 단일 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시글 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DELETE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/error</x:t>
-  </x:si>
-  <x:si>
-    <x:t>API</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EndPoints</x:t>
-  </x:si>
-  <x:si>
-    <x:t>어떤 데이터가 전달 될지 설계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>각 페이지로 이동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>에러 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/articles</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 가입</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/articles/{article-id}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시글 전체 리스트 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판 검색 전용 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시글 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/articles/search</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VIEW</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/articles/hashtag</x:t>
-  </x:si>
-  <x:si>
-    <x:t>id, pw, email, nickname, etc.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>id, pw</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/api/articles</x:t>
-  </x:si>
-  <x:si>
-    <x:t>댓글 단일 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/api/articles/{article-id}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>필터: 제목, 본문, id, 글쓴이, 해시태그</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PUT / PATCH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>제목, 본문, id, 해시태그</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/api/articleComments</x:t>
-  </x:si>
-  <x:si>
-    <x:t>필터: 본문</x:t>
-  </x:si>
-  <x:si>
-    <x:t>특정 게시글과 관련된 댓글 리스트 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/api/articles/{article-id}/articlecomments{article-comment-id}</x:t>
+    <x:t>/articles/search/hashtag</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -288,13 +288,41 @@
       </x:bottom>
     </x:border>
     <x:border>
-      <x:left style="medium">
-        <x:color auto="1"/>
+      <x:left>
+        <x:color rgb="ff000000"/>
       </x:left>
       <x:right>
-        <x:color auto="1"/>
+        <x:color rgb="ff000000"/>
       </x:right>
       <x:top style="medium">
+        <x:color auto="1"/>
+      </x:top>
+      <x:bottom>
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left>
+        <x:color rgb="ff000000"/>
+      </x:left>
+      <x:right style="medium">
+        <x:color auto="1"/>
+      </x:right>
+      <x:top style="medium">
+        <x:color auto="1"/>
+      </x:top>
+      <x:bottom>
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left>
+        <x:color rgb="ff000000"/>
+      </x:left>
+      <x:right style="medium">
+        <x:color auto="1"/>
+      </x:right>
+      <x:top>
         <x:color auto="1"/>
       </x:top>
       <x:bottom>
@@ -308,11 +336,11 @@
       <x:right>
         <x:color rgb="ff000000"/>
       </x:right>
-      <x:top style="medium">
+      <x:top>
         <x:color auto="1"/>
       </x:top>
-      <x:bottom>
-        <x:color rgb="ff000000"/>
+      <x:bottom style="medium">
+        <x:color auto="1"/>
       </x:bottom>
     </x:border>
     <x:border>
@@ -322,6 +350,20 @@
       <x:right style="medium">
         <x:color auto="1"/>
       </x:right>
+      <x:top>
+        <x:color auto="1"/>
+      </x:top>
+      <x:bottom style="medium">
+        <x:color auto="1"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left style="medium">
+        <x:color auto="1"/>
+      </x:left>
+      <x:right>
+        <x:color auto="1"/>
+      </x:right>
       <x:top style="medium">
         <x:color auto="1"/>
       </x:top>
@@ -344,52 +386,10 @@
       </x:bottom>
     </x:border>
     <x:border>
-      <x:left>
-        <x:color rgb="ff000000"/>
-      </x:left>
-      <x:right style="medium">
-        <x:color auto="1"/>
-      </x:right>
-      <x:top>
-        <x:color auto="1"/>
-      </x:top>
-      <x:bottom>
-        <x:color rgb="ff000000"/>
-      </x:bottom>
-    </x:border>
-    <x:border>
       <x:left style="medium">
         <x:color auto="1"/>
       </x:left>
       <x:right>
-        <x:color auto="1"/>
-      </x:right>
-      <x:top>
-        <x:color auto="1"/>
-      </x:top>
-      <x:bottom style="medium">
-        <x:color auto="1"/>
-      </x:bottom>
-    </x:border>
-    <x:border>
-      <x:left>
-        <x:color rgb="ff000000"/>
-      </x:left>
-      <x:right>
-        <x:color rgb="ff000000"/>
-      </x:right>
-      <x:top>
-        <x:color auto="1"/>
-      </x:top>
-      <x:bottom style="medium">
-        <x:color auto="1"/>
-      </x:bottom>
-    </x:border>
-    <x:border>
-      <x:left>
-        <x:color rgb="ff000000"/>
-      </x:left>
-      <x:right style="medium">
         <x:color auto="1"/>
       </x:right>
       <x:top>
@@ -412,19 +412,6 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" hs:applyExtension="1">
@@ -451,44 +438,64 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
         </x:xf>
       </mc:Choice>
       <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
@@ -502,39 +509,32 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </x:cellXfs>
   <x:cellStyles count="2">
     <x:cellStyle name="표준" xfId="0" builtinId="0" iLevel="0"/>
@@ -1258,7 +1258,7 @@
   <x:dimension ref="A1:E26"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <x:selection activeCell="K4" activeCellId="0" sqref="K4:K4"/>
+      <x:selection activeCell="I11" activeCellId="0" sqref="I11:I11"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="16.39999999999999857891"/>
@@ -1270,350 +1270,350 @@
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:5">
-      <x:c r="A1" s="1" t="s">
+      <x:c r="A1" s="18" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B1" s="18"/>
+      <x:c r="C1" s="18"/>
+      <x:c r="D1" s="18"/>
+      <x:c r="E1" s="18"/>
+    </x:row>
+    <x:row r="2" spans="1:5">
+      <x:c r="A2" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B2" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C2" s="1" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D2" s="1" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E2" s="1" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5" ht="16.75">
+      <x:c r="A3" s="19" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B3" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C3" s="3" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D3" s="3" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="E3" s="4" t="s">
+        <x:v>58</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5">
+      <x:c r="A4" s="20"/>
+      <x:c r="B4" s="5" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C4" s="5" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D4" s="5" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E4" s="6"/>
+    </x:row>
+    <x:row r="5" spans="1:5">
+      <x:c r="A5" s="20"/>
+      <x:c r="B5" s="5" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C5" s="5" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D5" s="5" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E5" s="6"/>
+    </x:row>
+    <x:row r="6" spans="1:5">
+      <x:c r="A6" s="20"/>
+      <x:c r="B6" s="5" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C6" s="5" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D6" s="5" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="E6" s="6"/>
+    </x:row>
+    <x:row r="7" spans="1:5">
+      <x:c r="A7" s="20"/>
+      <x:c r="B7" s="5" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C7" s="5" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D7" s="5" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E7" s="6"/>
+    </x:row>
+    <x:row r="8" spans="1:5">
+      <x:c r="A8" s="20"/>
+      <x:c r="B8" s="5" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C8" s="5" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D8" s="5" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E8" s="6"/>
+    </x:row>
+    <x:row r="9" spans="1:5">
+      <x:c r="A9" s="20"/>
+      <x:c r="B9" s="5" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C9" s="5" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D9" s="5" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="E9" s="6"/>
+    </x:row>
+    <x:row r="10" spans="1:5" ht="16.75">
+      <x:c r="A10" s="21"/>
+      <x:c r="B10" s="7" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C10" s="7" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D10" s="7" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="E10" s="8"/>
+    </x:row>
+    <x:row r="11" spans="1:1">
+      <x:c r="A11" s="2"/>
+    </x:row>
+    <x:row r="12" spans="1:5">
+      <x:c r="A12" s="2"/>
+      <x:c r="E12" t="s">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:5" ht="16.75">
+      <x:c r="A13" s="19" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B13" s="3" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C13" s="3" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D13" s="3" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E13" s="4" t="s">
+        <x:v>47</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:5">
+      <x:c r="A14" s="20"/>
+      <x:c r="B14" s="5" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C14" s="5" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D14" s="5" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E14" s="6" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:5">
+      <x:c r="A15" s="20"/>
+      <x:c r="B15" s="15" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="C15" s="15" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D15" s="15" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="E15" s="16" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:5">
+      <x:c r="A16" s="20"/>
+      <x:c r="B16" s="15" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C16" s="15" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D16" s="15" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="E16" s="16"/>
+    </x:row>
+    <x:row r="17" spans="1:5">
+      <x:c r="A17" s="20"/>
+      <x:c r="B17" s="15" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="C17" s="15" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D17" s="15" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E17" s="16" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:5">
+      <x:c r="A18" s="20"/>
+      <x:c r="B18" s="17" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C18" s="15" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="D18" s="15" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="B1" s="1"/>
-      <x:c r="C1" s="1"/>
-      <x:c r="D1" s="1"/>
-      <x:c r="E1" s="1"/>
-    </x:row>
-    <x:row r="2" spans="1:5">
-      <x:c r="A2" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B2" s="2" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="C2" s="2" t="s">
+      <x:c r="E18" s="16" t="s">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:5">
+      <x:c r="A19" s="20"/>
+      <x:c r="B19" s="17" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C19" s="15" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D19" s="15" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="E19" s="16" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:5">
+      <x:c r="A20" s="20"/>
+      <x:c r="B20" s="9" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="D2" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E2" s="2" t="s">
+      <x:c r="C20" s="9" t="s">
         <x:v>16</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5">
-      <x:c r="A3" s="4" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="B3" s="5" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="C3" s="5" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D3" s="5" t="s">
+      <x:c r="D20" s="9" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="E20" s="10"/>
+    </x:row>
+    <x:row r="21" spans="1:5">
+      <x:c r="A21" s="20"/>
+      <x:c r="B21" s="9" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="E3" s="6" t="s">
-        <x:v>39</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5">
-      <x:c r="A4" s="7"/>
-      <x:c r="B4" s="8" t="s">
+      <x:c r="C21" s="9" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D21" s="9" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="E21" s="10"/>
+    </x:row>
+    <x:row r="22" spans="1:5">
+      <x:c r="A22" s="20"/>
+      <x:c r="B22" s="11" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C22" s="11" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D22" s="11" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E22" s="12" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:5">
+      <x:c r="A23" s="20"/>
+      <x:c r="B23" s="11" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C23" s="11" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D23" s="11" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E23" s="12"/>
+    </x:row>
+    <x:row r="24" spans="1:5">
+      <x:c r="A24" s="20"/>
+      <x:c r="B24" s="11" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C24" s="11" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D24" s="11" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="E24" s="12" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:5">
+      <x:c r="A25" s="20"/>
+      <x:c r="B25" s="11" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C25" s="11" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="D25" s="11" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E25" s="12" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:5" ht="16.75">
+      <x:c r="A26" s="21"/>
+      <x:c r="B26" s="13" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C26" s="13" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D26" s="13" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="E26" s="14" t="s">
         <x:v>34</x:v>
-      </x:c>
-      <x:c r="C4" s="8" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D4" s="8" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="E4" s="9"/>
-    </x:row>
-    <x:row r="5" spans="1:5">
-      <x:c r="A5" s="7"/>
-      <x:c r="B5" s="8" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="C5" s="8" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D5" s="8" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="E5" s="9"/>
-    </x:row>
-    <x:row r="6" spans="1:5">
-      <x:c r="A6" s="7"/>
-      <x:c r="B6" s="8" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C6" s="8" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D6" s="8" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="E6" s="9"/>
-    </x:row>
-    <x:row r="7" spans="1:5">
-      <x:c r="A7" s="7"/>
-      <x:c r="B7" s="8" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C7" s="8" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D7" s="8" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="E7" s="9"/>
-    </x:row>
-    <x:row r="8" spans="1:5">
-      <x:c r="A8" s="7"/>
-      <x:c r="B8" s="8" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C8" s="8" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D8" s="8" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="E8" s="9"/>
-    </x:row>
-    <x:row r="9" spans="1:5">
-      <x:c r="A9" s="7"/>
-      <x:c r="B9" s="8" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="C9" s="8" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D9" s="8" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="E9" s="9"/>
-    </x:row>
-    <x:row r="10" spans="1:5">
-      <x:c r="A10" s="10"/>
-      <x:c r="B10" s="11" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="C10" s="11" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D10" s="11" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E10" s="12"/>
-    </x:row>
-    <x:row r="11" spans="1:1">
-      <x:c r="A11" s="3"/>
-    </x:row>
-    <x:row r="12" spans="1:5">
-      <x:c r="A12" s="3"/>
-      <x:c r="E12" t="s">
-        <x:v>37</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5">
-      <x:c r="A13" s="4" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="B13" s="5" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C13" s="5" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="D13" s="5" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="E13" s="6" t="s">
-        <x:v>51</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:5">
-      <x:c r="A14" s="7"/>
-      <x:c r="B14" s="8" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="C14" s="8" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="D14" s="8" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="E14" s="9" t="s">
-        <x:v>52</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:5">
-      <x:c r="A15" s="7"/>
-      <x:c r="B15" s="19" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="C15" s="19" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D15" s="19" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="E15" s="20" t="s">
-        <x:v>56</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:5">
-      <x:c r="A16" s="7"/>
-      <x:c r="B16" s="19" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="C16" s="19" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D16" s="19" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="E16" s="20"/>
-    </x:row>
-    <x:row r="17" spans="1:5">
-      <x:c r="A17" s="7"/>
-      <x:c r="B17" s="19" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="C17" s="19" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="D17" s="19" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E17" s="20" t="s">
-        <x:v>58</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:5">
-      <x:c r="A18" s="7"/>
-      <x:c r="B18" s="21" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="C18" s="19" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="D18" s="19" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="E18" s="20" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:5">
-      <x:c r="A19" s="7"/>
-      <x:c r="B19" s="21" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="C19" s="19" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="D19" s="19" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E19" s="20" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:5">
-      <x:c r="A20" s="7"/>
-      <x:c r="B20" s="13" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="C20" s="13" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D20" s="13" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="E20" s="14"/>
-    </x:row>
-    <x:row r="21" spans="1:5">
-      <x:c r="A21" s="7"/>
-      <x:c r="B21" s="13" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="C21" s="13" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D21" s="13" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="E21" s="14"/>
-    </x:row>
-    <x:row r="22" spans="1:5">
-      <x:c r="A22" s="7"/>
-      <x:c r="B22" s="15" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="C22" s="15" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D22" s="15" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="E22" s="16" t="s">
-        <x:v>60</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:5" ht="16.75">
-      <x:c r="A23" s="7"/>
-      <x:c r="B23" s="15" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="C23" s="15" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D23" s="15" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E23" s="16"/>
-    </x:row>
-    <x:row r="24" spans="1:5">
-      <x:c r="A24" s="7"/>
-      <x:c r="B24" s="15" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="C24" s="15" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="D24" s="15" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="E24" s="16" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:5">
-      <x:c r="A25" s="7"/>
-      <x:c r="B25" s="15" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="C25" s="15" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="D25" s="15" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="E25" s="16" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:5">
-      <x:c r="A26" s="10"/>
-      <x:c r="B26" s="17" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="C26" s="17" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="D26" s="17" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E26" s="18" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1622,7 +1622,7 @@
     <x:mergeCell ref="A3:A10"/>
     <x:mergeCell ref="A13:A26"/>
   </x:mergeCells>
-  <x:pageMargins left="0.74805557727813720703" right="0.74805557727813720703" top="0.98430556058883666992" bottom="0.98430556058883666992" header="0.51166665554046630859" footer="0.51166665554046630859"/>
+  <x:pageMargins left="0.74805557727813720703" right="0.74805557727813720703" top="0.98430556058883666992" bottom="0.98430556058883666992" header="0.51152777671813964844" footer="0.51152777671813964844"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>